<commit_message>
Updating the project plan with the delivered tasks
</commit_message>
<xml_diff>
--- a/SWE/SW deliveries log/PP/SWE_PO1_Digital_Calculator_ITI_41.xlsx
+++ b/SWE/SW deliveries log/PP/SWE_PO1_Digital_Calculator_ITI_41.xlsx
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="72">
   <si>
     <t>Sovy - Digital Calculator PO1_DGC</t>
   </si>
@@ -230,6 +230,18 @@
     <t>Third Week's Plan</t>
   </si>
   <si>
+    <t>Task 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Abdullah </t>
+  </si>
+  <si>
+    <t>- Project Plan</t>
+  </si>
+  <si>
+    <t>- Add project plan for week 3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Task 1 </t>
   </si>
   <si>
@@ -245,7 +257,7 @@
     <t>Task 2</t>
   </si>
   <si>
-    <t xml:space="preserve">Abdullah </t>
+    <t>Nour</t>
   </si>
   <si>
     <t>- Modify HSI</t>
@@ -257,9 +269,6 @@
     <t>Task 3</t>
   </si>
   <si>
-    <t xml:space="preserve"> Abdullah </t>
-  </si>
-  <si>
     <t>- Draw the SRS Context diagram</t>
   </si>
   <si>
@@ -288,9 +297,6 @@
   </si>
   <si>
     <t>Task 5</t>
-  </si>
-  <si>
-    <t>Nour</t>
   </si>
   <si>
     <t xml:space="preserve">- Recolour all the documnets </t>
@@ -335,7 +341,7 @@
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="166" formatCode="h:mm am/pm"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="18">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -420,12 +426,8 @@
       <sz val="12.0"/>
       <name val="Roboto"/>
     </font>
-    <font>
-      <color rgb="FF434343"/>
-      <name val="Roboto"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -454,6 +456,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
   </fills>
@@ -618,7 +626,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="114">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -844,75 +852,91 @@
     <xf borderId="16" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="11" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="2" fontId="14" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="3" fontId="14" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="4" fontId="14" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="3" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="5" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="5" fontId="13" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="5" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="12" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf borderId="6" fillId="5" fontId="14" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="5" fontId="14" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="3" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="5" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="5" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="4" fontId="13" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="4" fontId="14" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="4" fontId="14" numFmtId="165" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="6" fillId="5" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="6" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="6" fillId="2" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="6" fillId="3" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="6" fillId="5" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf borderId="6" fillId="5" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="5" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="6" fillId="4" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="6" fillId="4" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="6" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf borderId="6" fillId="5" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="6" fillId="5" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="4" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="4" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf borderId="6" fillId="3" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="6" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="6" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="5" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
+    <xf borderId="6" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
@@ -920,9 +944,6 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1464,466 +1485,532 @@
       <c r="K17" s="13"/>
     </row>
     <row r="18" ht="22.5" customHeight="1">
-      <c r="A18" s="42"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="40" t="s">
+      <c r="A18" s="20"/>
+      <c r="B18" s="75"/>
+      <c r="C18" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="E18" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="F18" s="17" t="s">
+      <c r="F18" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="G18" s="17" t="s">
+      <c r="G18" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="H18" s="17" t="s">
+      <c r="H18" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="I18" s="17" t="s">
+      <c r="I18" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="J18" s="17" t="s">
+      <c r="J18" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="K18" s="17" t="s">
+      <c r="K18" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="L18" s="18"/>
-      <c r="M18" s="18"/>
-      <c r="N18" s="18"/>
-      <c r="O18" s="75"/>
-      <c r="P18" s="75"/>
+      <c r="L18" s="77"/>
+      <c r="M18" s="77"/>
+      <c r="N18" s="77"/>
+      <c r="O18" s="78"/>
+      <c r="P18" s="78"/>
     </row>
     <row r="19" ht="22.5" customHeight="1">
-      <c r="A19" s="42"/>
-      <c r="B19" s="43" t="s">
+      <c r="A19" s="20"/>
+      <c r="B19" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="76" t="s">
+      <c r="C19" s="80" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="77" t="s">
+      <c r="D19" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="77" t="s">
+      <c r="E19" s="80" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="53">
+      <c r="F19" s="81">
         <v>44259.0</v>
       </c>
-      <c r="G19" s="53">
+      <c r="G19" s="81">
         <v>44259.0</v>
       </c>
-      <c r="H19" s="53">
+      <c r="H19" s="81">
         <v>44259.0</v>
       </c>
-      <c r="I19" s="53">
+      <c r="I19" s="81">
         <v>44259.0</v>
       </c>
-      <c r="J19" s="78">
+      <c r="J19" s="82">
+        <v>2.0</v>
+      </c>
+      <c r="K19" s="82">
+        <v>2.0</v>
+      </c>
+      <c r="L19" s="83"/>
+      <c r="M19" s="83"/>
+      <c r="N19" s="83"/>
+      <c r="O19" s="84"/>
+      <c r="P19" s="84"/>
+    </row>
+    <row r="20" ht="22.5" customHeight="1">
+      <c r="A20" s="20"/>
+      <c r="B20" s="85" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="86" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="86" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" s="86" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="81">
+        <v>44259.0</v>
+      </c>
+      <c r="G20" s="81">
+        <v>44259.0</v>
+      </c>
+      <c r="H20" s="81">
+        <v>44259.0</v>
+      </c>
+      <c r="I20" s="81">
+        <v>44259.0</v>
+      </c>
+      <c r="J20" s="87">
         <v>0.5</v>
       </c>
-      <c r="K19" s="79">
+      <c r="K20" s="87">
         <v>0.5</v>
       </c>
-      <c r="L19" s="80"/>
-      <c r="M19" s="80"/>
-      <c r="N19" s="80"/>
-      <c r="O19" s="33"/>
-      <c r="P19" s="33"/>
-    </row>
-    <row r="20" ht="22.5" customHeight="1">
-      <c r="A20" s="42"/>
-      <c r="B20" s="49" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="65" t="s">
+      <c r="L20" s="83"/>
+      <c r="M20" s="83"/>
+      <c r="N20" s="83"/>
+      <c r="O20" s="84"/>
+      <c r="P20" s="84"/>
+    </row>
+    <row r="21" ht="22.5" customHeight="1">
+      <c r="A21" s="20"/>
+      <c r="B21" s="85" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="88" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="88" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="88" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21" s="89">
+        <v>44259.0</v>
+      </c>
+      <c r="G21" s="89">
+        <v>44259.0</v>
+      </c>
+      <c r="H21" s="89">
+        <v>44259.0</v>
+      </c>
+      <c r="I21" s="89">
+        <v>44259.0</v>
+      </c>
+      <c r="J21" s="90">
+        <v>0.5</v>
+      </c>
+      <c r="K21" s="90">
+        <v>0.5</v>
+      </c>
+      <c r="L21" s="91"/>
+      <c r="M21" s="92"/>
+      <c r="N21" s="92"/>
+      <c r="O21" s="78"/>
+      <c r="P21" s="78"/>
+    </row>
+    <row r="22" ht="22.5" customHeight="1">
+      <c r="A22" s="20"/>
+      <c r="B22" s="85" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="93" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="86" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" s="86" t="s">
+        <v>52</v>
+      </c>
+      <c r="F22" s="81">
+        <v>44259.0</v>
+      </c>
+      <c r="G22" s="81">
+        <v>44260.0</v>
+      </c>
+      <c r="H22" s="81">
+        <v>44259.0</v>
+      </c>
+      <c r="I22" s="81">
+        <v>44260.0</v>
+      </c>
+      <c r="J22" s="87">
+        <v>4.0</v>
+      </c>
+      <c r="K22" s="87">
+        <v>4.0</v>
+      </c>
+      <c r="L22" s="84"/>
+      <c r="M22" s="84"/>
+      <c r="N22" s="84"/>
+      <c r="O22" s="84"/>
+      <c r="P22" s="84"/>
+    </row>
+    <row r="23" ht="22.5" customHeight="1">
+      <c r="A23" s="20"/>
+      <c r="B23" s="85" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="88" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="88" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="88" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" s="89">
+        <v>44259.0</v>
+      </c>
+      <c r="G23" s="89">
+        <v>44260.0</v>
+      </c>
+      <c r="H23" s="89">
+        <v>44259.0</v>
+      </c>
+      <c r="I23" s="89">
+        <v>44260.0</v>
+      </c>
+      <c r="J23" s="90">
+        <v>4.0</v>
+      </c>
+      <c r="K23" s="94">
+        <v>4.0</v>
+      </c>
+      <c r="L23" s="78"/>
+      <c r="M23" s="78"/>
+      <c r="N23" s="78"/>
+      <c r="O23" s="78"/>
+      <c r="P23" s="78"/>
+    </row>
+    <row r="24" ht="22.5" customHeight="1">
+      <c r="A24" s="95"/>
+      <c r="B24" s="85" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="86" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="57" t="s">
-        <v>44</v>
-      </c>
-      <c r="E20" s="57" t="s">
-        <v>45</v>
-      </c>
-      <c r="F20" s="46">
+      <c r="D24" s="86" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="86" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" s="81">
+        <v>44260.0</v>
+      </c>
+      <c r="G24" s="81">
+        <v>44261.0</v>
+      </c>
+      <c r="H24" s="81">
+        <v>44262.0</v>
+      </c>
+      <c r="I24" s="81">
+        <v>44262.0</v>
+      </c>
+      <c r="J24" s="96">
+        <v>4.0</v>
+      </c>
+      <c r="K24" s="97">
+        <v>7.0</v>
+      </c>
+      <c r="L24" s="84"/>
+      <c r="M24" s="84"/>
+      <c r="N24" s="84"/>
+      <c r="O24" s="84"/>
+      <c r="P24" s="84"/>
+    </row>
+    <row r="25" ht="22.5" customHeight="1">
+      <c r="A25" s="98"/>
+      <c r="B25" s="85" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="99" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" s="88" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="88" t="s">
+        <v>57</v>
+      </c>
+      <c r="F25" s="89">
+        <v>44260.0</v>
+      </c>
+      <c r="G25" s="89">
+        <v>44261.0</v>
+      </c>
+      <c r="H25" s="89">
+        <v>44262.0</v>
+      </c>
+      <c r="I25" s="89">
+        <v>44262.0</v>
+      </c>
+      <c r="J25" s="90">
+        <v>4.0</v>
+      </c>
+      <c r="K25" s="100">
+        <v>7.0</v>
+      </c>
+      <c r="L25" s="78"/>
+      <c r="M25" s="78"/>
+      <c r="N25" s="78"/>
+      <c r="O25" s="78"/>
+      <c r="P25" s="78"/>
+    </row>
+    <row r="26" ht="22.5" customHeight="1">
+      <c r="A26" s="20"/>
+      <c r="B26" s="85" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="86" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="86" t="s">
+        <v>61</v>
+      </c>
+      <c r="E26" s="86" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26" s="81">
         <v>44259.0</v>
       </c>
-      <c r="G20" s="46">
-        <v>44259.0</v>
-      </c>
-      <c r="H20" s="46">
-        <v>44259.0</v>
-      </c>
-      <c r="I20" s="46">
-        <v>44259.0</v>
-      </c>
-      <c r="J20" s="47">
+      <c r="G26" s="81">
+        <v>44260.0</v>
+      </c>
+      <c r="H26" s="81">
+        <v>44260.0</v>
+      </c>
+      <c r="I26" s="101"/>
+      <c r="J26" s="87">
+        <v>1.0</v>
+      </c>
+      <c r="K26" s="102"/>
+      <c r="L26" s="84"/>
+      <c r="M26" s="84"/>
+      <c r="N26" s="84"/>
+      <c r="O26" s="84"/>
+      <c r="P26" s="84"/>
+    </row>
+    <row r="27" ht="22.5" customHeight="1">
+      <c r="A27" s="98"/>
+      <c r="B27" s="85" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="103" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="88" t="s">
+        <v>65</v>
+      </c>
+      <c r="E27" s="88" t="s">
+        <v>66</v>
+      </c>
+      <c r="F27" s="89">
+        <v>44261.0</v>
+      </c>
+      <c r="G27" s="89">
+        <v>44262.0</v>
+      </c>
+      <c r="H27" s="89">
+        <v>44262.0</v>
+      </c>
+      <c r="I27" s="104"/>
+      <c r="J27" s="90">
+        <v>1.0</v>
+      </c>
+      <c r="K27" s="100">
+        <v>2.0</v>
+      </c>
+      <c r="L27" s="78"/>
+      <c r="M27" s="78"/>
+      <c r="N27" s="78"/>
+      <c r="O27" s="78"/>
+      <c r="P27" s="78"/>
+    </row>
+    <row r="28" ht="22.5" customHeight="1">
+      <c r="A28" s="20"/>
+      <c r="B28" s="85" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="86" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="86" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" s="86" t="s">
+        <v>62</v>
+      </c>
+      <c r="F28" s="81">
+        <v>44260.0</v>
+      </c>
+      <c r="G28" s="81">
+        <v>44261.0</v>
+      </c>
+      <c r="H28" s="81">
+        <v>44261.0</v>
+      </c>
+      <c r="I28" s="101"/>
+      <c r="J28" s="87">
+        <v>1.0</v>
+      </c>
+      <c r="K28" s="102"/>
+      <c r="L28" s="84"/>
+      <c r="M28" s="84"/>
+      <c r="N28" s="84"/>
+      <c r="O28" s="84"/>
+      <c r="P28" s="84"/>
+    </row>
+    <row r="29" ht="22.5" customHeight="1">
+      <c r="A29" s="98"/>
+      <c r="B29" s="85" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="99" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29" s="88" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29" s="88" t="s">
+        <v>66</v>
+      </c>
+      <c r="F29" s="89">
+        <v>44261.0</v>
+      </c>
+      <c r="G29" s="89">
+        <v>44262.0</v>
+      </c>
+      <c r="H29" s="89">
+        <v>44262.0</v>
+      </c>
+      <c r="I29" s="101"/>
+      <c r="J29" s="90">
+        <v>3.0</v>
+      </c>
+      <c r="K29" s="104"/>
+      <c r="L29" s="78"/>
+      <c r="M29" s="78"/>
+      <c r="N29" s="78"/>
+      <c r="O29" s="78"/>
+      <c r="P29" s="78"/>
+    </row>
+    <row r="30" ht="22.5" customHeight="1">
+      <c r="A30" s="20"/>
+      <c r="B30" s="85" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" s="86" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="86" t="s">
+        <v>70</v>
+      </c>
+      <c r="E30" s="86" t="s">
+        <v>71</v>
+      </c>
+      <c r="F30" s="81">
+        <v>44261.0</v>
+      </c>
+      <c r="G30" s="81">
+        <v>44262.0</v>
+      </c>
+      <c r="H30" s="81">
+        <v>44262.0</v>
+      </c>
+      <c r="I30" s="101"/>
+      <c r="J30" s="87">
         <v>0.5</v>
       </c>
-      <c r="K20" s="48">
-        <v>0.5</v>
-      </c>
-      <c r="L20" s="81"/>
-      <c r="M20" s="23"/>
-      <c r="N20" s="23"/>
-      <c r="O20" s="26"/>
-      <c r="P20" s="26"/>
-    </row>
-    <row r="21" ht="22.5" customHeight="1">
-      <c r="A21" s="42"/>
-      <c r="B21" s="49" t="s">
-        <v>46</v>
-      </c>
-      <c r="C21" s="82" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" s="51" t="s">
-        <v>48</v>
-      </c>
-      <c r="E21" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="F21" s="53">
-        <v>44259.0</v>
-      </c>
-      <c r="G21" s="53">
-        <v>44260.0</v>
-      </c>
-      <c r="H21" s="53">
-        <v>44259.0</v>
-      </c>
-      <c r="I21" s="53">
-        <v>44260.0</v>
-      </c>
-      <c r="J21" s="54">
-        <v>4.0</v>
-      </c>
-      <c r="K21" s="55"/>
-      <c r="L21" s="64"/>
-      <c r="M21" s="64"/>
-      <c r="N21" s="64"/>
-      <c r="O21" s="64"/>
-      <c r="P21" s="64"/>
-    </row>
-    <row r="22" ht="22.5" customHeight="1">
-      <c r="A22" s="42"/>
-      <c r="B22" s="49" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" s="65" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="57" t="s">
-        <v>48</v>
-      </c>
-      <c r="E22" s="83" t="s">
-        <v>49</v>
-      </c>
-      <c r="F22" s="46">
-        <v>44259.0</v>
-      </c>
-      <c r="G22" s="46">
-        <v>44260.0</v>
-      </c>
-      <c r="H22" s="46">
-        <v>44259.0</v>
-      </c>
-      <c r="I22" s="46">
-        <v>44260.0</v>
-      </c>
-      <c r="J22" s="59">
-        <v>4.0</v>
-      </c>
-      <c r="K22" s="68"/>
-      <c r="L22" s="37"/>
-      <c r="M22" s="37"/>
-      <c r="N22" s="37"/>
-      <c r="O22" s="37"/>
-      <c r="P22" s="37"/>
-    </row>
-    <row r="23" ht="22.5" customHeight="1">
-      <c r="A23" s="84"/>
-      <c r="B23" s="85" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="76" t="s">
-        <v>39</v>
-      </c>
-      <c r="D23" s="86" t="s">
-        <v>53</v>
-      </c>
-      <c r="E23" s="62" t="s">
-        <v>54</v>
-      </c>
-      <c r="F23" s="53">
-        <v>44260.0</v>
-      </c>
-      <c r="G23" s="53">
-        <v>44261.0</v>
-      </c>
-      <c r="H23" s="87"/>
-      <c r="I23" s="87"/>
-      <c r="J23" s="88">
-        <v>4.0</v>
-      </c>
-      <c r="K23" s="87"/>
-      <c r="L23" s="87"/>
-      <c r="M23" s="87"/>
-      <c r="N23" s="87"/>
-      <c r="O23" s="87"/>
-      <c r="P23" s="87"/>
-    </row>
-    <row r="24" ht="22.5" customHeight="1">
-      <c r="A24" s="89"/>
-      <c r="B24" s="90" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" s="91" t="s">
-        <v>56</v>
-      </c>
-      <c r="D24" s="92" t="s">
-        <v>53</v>
-      </c>
-      <c r="E24" s="67" t="s">
-        <v>54</v>
-      </c>
-      <c r="F24" s="46">
-        <v>44260.0</v>
-      </c>
-      <c r="G24" s="46">
-        <v>44261.0</v>
-      </c>
-      <c r="H24" s="93"/>
-      <c r="I24" s="93"/>
-      <c r="J24" s="59">
-        <v>4.0</v>
-      </c>
-      <c r="K24" s="94"/>
-      <c r="L24" s="93"/>
-      <c r="M24" s="93"/>
-      <c r="N24" s="93"/>
-      <c r="O24" s="93"/>
-      <c r="P24" s="93"/>
-    </row>
-    <row r="25" ht="22.5" customHeight="1">
-      <c r="A25" s="42"/>
-      <c r="B25" s="49" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="D25" s="95" t="s">
-        <v>59</v>
-      </c>
-      <c r="E25" s="62" t="s">
-        <v>60</v>
-      </c>
-      <c r="F25" s="53">
-        <v>44259.0</v>
-      </c>
-      <c r="G25" s="53">
-        <v>44260.0</v>
-      </c>
-      <c r="H25" s="96"/>
-      <c r="I25" s="96"/>
-      <c r="J25" s="54">
-        <v>2.0</v>
-      </c>
-      <c r="K25" s="63"/>
-      <c r="L25" s="64"/>
-      <c r="M25" s="64"/>
-      <c r="N25" s="64"/>
-      <c r="O25" s="64"/>
-      <c r="P25" s="64"/>
-    </row>
-    <row r="26" ht="22.5" customHeight="1">
-      <c r="A26" s="89"/>
-      <c r="B26" s="90" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" s="91" t="s">
-        <v>62</v>
-      </c>
-      <c r="D26" s="57" t="s">
-        <v>63</v>
-      </c>
-      <c r="E26" s="67" t="s">
-        <v>64</v>
-      </c>
-      <c r="F26" s="46">
-        <v>44261.0</v>
-      </c>
-      <c r="G26" s="46">
-        <v>44262.0</v>
-      </c>
-      <c r="H26" s="93"/>
-      <c r="I26" s="93"/>
-      <c r="J26" s="59">
-        <v>1.0</v>
-      </c>
-      <c r="K26" s="94"/>
-      <c r="L26" s="93"/>
-      <c r="M26" s="93"/>
-      <c r="N26" s="93"/>
-      <c r="O26" s="93"/>
-      <c r="P26" s="93"/>
-    </row>
-    <row r="27" ht="22.5" customHeight="1">
-      <c r="A27" s="42"/>
-      <c r="B27" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="C27" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="D27" s="95" t="s">
-        <v>65</v>
-      </c>
-      <c r="E27" s="62" t="s">
-        <v>60</v>
-      </c>
-      <c r="F27" s="53">
-        <v>44260.0</v>
-      </c>
-      <c r="G27" s="53">
-        <v>44261.0</v>
-      </c>
-      <c r="H27" s="96"/>
-      <c r="I27" s="96"/>
-      <c r="J27" s="54">
-        <v>1.0</v>
-      </c>
-      <c r="K27" s="63"/>
-      <c r="L27" s="64"/>
-      <c r="M27" s="64"/>
-      <c r="N27" s="64"/>
-      <c r="O27" s="64"/>
-      <c r="P27" s="64"/>
-    </row>
-    <row r="28" ht="22.5" customHeight="1">
-      <c r="A28" s="89"/>
-      <c r="B28" s="90" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" s="91" t="s">
-        <v>62</v>
-      </c>
-      <c r="D28" s="57" t="s">
-        <v>66</v>
-      </c>
-      <c r="E28" s="67" t="s">
-        <v>64</v>
-      </c>
-      <c r="F28" s="46">
-        <v>44261.0</v>
-      </c>
-      <c r="G28" s="46">
-        <v>44262.0</v>
-      </c>
-      <c r="H28" s="93"/>
-      <c r="I28" s="93"/>
-      <c r="J28" s="59">
-        <v>3.0</v>
-      </c>
-      <c r="K28" s="94"/>
-      <c r="L28" s="93"/>
-      <c r="M28" s="93"/>
-      <c r="N28" s="93"/>
-      <c r="O28" s="93"/>
-      <c r="P28" s="93"/>
-    </row>
-    <row r="29" ht="22.5" customHeight="1">
-      <c r="A29" s="42"/>
-      <c r="B29" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="C29" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="D29" s="95" t="s">
-        <v>68</v>
-      </c>
-      <c r="E29" s="62" t="s">
-        <v>69</v>
-      </c>
-      <c r="F29" s="53">
-        <v>44261.0</v>
-      </c>
-      <c r="G29" s="53">
-        <v>44262.0</v>
-      </c>
-      <c r="H29" s="96"/>
-      <c r="I29" s="96"/>
-      <c r="J29" s="54">
-        <v>1.5</v>
-      </c>
-      <c r="K29" s="63"/>
-      <c r="L29" s="64"/>
-      <c r="M29" s="64"/>
-      <c r="N29" s="64"/>
-      <c r="O29" s="64"/>
-      <c r="P29" s="64"/>
-    </row>
-    <row r="30" ht="22.5" customHeight="1">
-      <c r="A30" s="97"/>
-      <c r="B30" s="98"/>
-      <c r="C30" s="99"/>
-      <c r="D30" s="99"/>
-      <c r="E30" s="99"/>
-      <c r="F30" s="99"/>
-      <c r="G30" s="100"/>
-      <c r="H30" s="100"/>
-      <c r="I30" s="98"/>
-      <c r="J30" s="99"/>
-      <c r="K30" s="99"/>
-      <c r="L30" s="99"/>
-      <c r="M30" s="99"/>
-      <c r="N30" s="101"/>
-      <c r="O30" s="100"/>
-      <c r="P30" s="100"/>
+      <c r="K30" s="102"/>
+      <c r="L30" s="84"/>
+      <c r="M30" s="84"/>
+      <c r="N30" s="84"/>
+      <c r="O30" s="84"/>
+      <c r="P30" s="84"/>
     </row>
     <row r="31" ht="22.5" customHeight="1">
-      <c r="A31" s="97"/>
-      <c r="B31" s="98"/>
-      <c r="C31" s="99"/>
-      <c r="D31" s="99"/>
-      <c r="E31" s="99"/>
-      <c r="F31" s="99"/>
-      <c r="G31" s="100"/>
-      <c r="H31" s="100"/>
-      <c r="I31" s="98"/>
-      <c r="J31" s="99"/>
-      <c r="K31" s="99"/>
-      <c r="L31" s="99"/>
-      <c r="M31" s="99"/>
-      <c r="N31" s="100"/>
-      <c r="O31" s="100"/>
-      <c r="P31" s="100"/>
-    </row>
-    <row r="32" ht="6.0" customHeight="1">
-      <c r="A32" s="102"/>
-      <c r="B32" s="103"/>
-      <c r="C32" s="102"/>
-      <c r="D32" s="102"/>
-      <c r="E32" s="102"/>
-      <c r="F32" s="102"/>
-      <c r="G32" s="102"/>
-      <c r="H32" s="102"/>
-      <c r="I32" s="102"/>
-      <c r="J32" s="104"/>
-      <c r="K32" s="104"/>
-      <c r="L32" s="102"/>
-      <c r="M32" s="102"/>
-      <c r="N32" s="102"/>
-      <c r="O32" s="102"/>
-      <c r="P32" s="102"/>
+      <c r="A31" s="105"/>
+      <c r="B31" s="106"/>
+      <c r="C31" s="106"/>
+      <c r="D31" s="106"/>
+      <c r="E31" s="106"/>
+      <c r="F31" s="106"/>
+      <c r="G31" s="106"/>
+      <c r="H31" s="106"/>
+      <c r="I31" s="106"/>
+      <c r="J31" s="106"/>
+      <c r="K31" s="106"/>
+      <c r="L31" s="107"/>
+      <c r="M31" s="107"/>
+      <c r="N31" s="107"/>
+      <c r="O31" s="107"/>
+      <c r="P31" s="107"/>
+    </row>
+    <row r="32" ht="22.5" customHeight="1">
+      <c r="A32" s="105"/>
+      <c r="B32" s="108"/>
+      <c r="C32" s="109"/>
+      <c r="D32" s="109"/>
+      <c r="E32" s="109"/>
+      <c r="F32" s="109"/>
+      <c r="G32" s="110"/>
+      <c r="H32" s="110"/>
+      <c r="I32" s="108"/>
+      <c r="J32" s="109"/>
+      <c r="K32" s="109"/>
+      <c r="L32" s="109"/>
+      <c r="M32" s="109"/>
+      <c r="N32" s="110"/>
+      <c r="O32" s="110"/>
+      <c r="P32" s="110"/>
+    </row>
+    <row r="33" ht="6.0" customHeight="1">
+      <c r="A33" s="111"/>
+      <c r="B33" s="112"/>
+      <c r="C33" s="111"/>
+      <c r="D33" s="111"/>
+      <c r="E33" s="111"/>
+      <c r="F33" s="111"/>
+      <c r="G33" s="111"/>
+      <c r="H33" s="111"/>
+      <c r="I33" s="111"/>
+      <c r="J33" s="113"/>
+      <c r="K33" s="113"/>
+      <c r="L33" s="111"/>
+      <c r="M33" s="111"/>
+      <c r="N33" s="111"/>
+      <c r="O33" s="111"/>
+      <c r="P33" s="111"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>

<commit_message>
Updating the project plan with lastly delivered documents
</commit_message>
<xml_diff>
--- a/SWE/SW deliveries log/PP/SWE_PO1_Digital_Calculator_ITI_41.xlsx
+++ b/SWE/SW deliveries log/PP/SWE_PO1_Digital_Calculator_ITI_41.xlsx
@@ -1519,7 +1519,7 @@
       <c r="J25" s="72">
         <v>1.0</v>
       </c>
-      <c r="K25" s="58"/>
+      <c r="K25" s="71"/>
       <c r="L25" s="58"/>
       <c r="M25" s="58"/>
       <c r="N25" s="58"/>
@@ -1631,7 +1631,9 @@
       <c r="J28" s="77">
         <v>3.0</v>
       </c>
-      <c r="K28" s="52"/>
+      <c r="K28" s="70">
+        <v>2.0</v>
+      </c>
       <c r="L28" s="52"/>
       <c r="M28" s="52"/>
       <c r="N28" s="52"/>
@@ -1667,7 +1669,9 @@
       <c r="J29" s="72">
         <v>0.5</v>
       </c>
-      <c r="K29" s="58"/>
+      <c r="K29" s="67">
+        <v>0.5</v>
+      </c>
       <c r="L29" s="58"/>
       <c r="M29" s="58"/>
       <c r="N29" s="58"/>

</xml_diff>

<commit_message>
Project Plan for week 4
</commit_message>
<xml_diff>
--- a/SWE/SW deliveries log/PP/SWE_PO1_Digital_Calculator_ITI_41.xlsx
+++ b/SWE/SW deliveries log/PP/SWE_PO1_Digital_Calculator_ITI_41.xlsx
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="93">
   <si>
     <t>Sovy - Digital Calculator PO1_DGC</t>
   </si>
@@ -337,17 +337,73 @@
   <si>
     <t xml:space="preserve">- Review on the new added reqs in the RTM </t>
   </si>
+  <si>
+    <t>Forth Week's Plan</t>
+  </si>
+  <si>
+    <t>- Add project plan for week 4</t>
+  </si>
+  <si>
+    <t>Habiba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-Modify the SRS requirments </t>
+  </si>
+  <si>
+    <t>-Modify your SRS requirments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abdullah  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Modify the context diagram </t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Modify the context diagram in the SRS according to the last review </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hossam </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-make the RTM more readable, and add the last modifications as per the SRS,HSI and CRS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nour </t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Modify the CRS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Modify the CRS as per the last review </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-Modify the HSI </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-Add the lcd initilization sequence,and update the document as per the last review </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nihal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andrew </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-Review the SRS requirements </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-Review the SRS context diagram </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m&quot;/&quot;d"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="166" formatCode="h:mm am/pm"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="16">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -422,16 +478,6 @@
       <color rgb="FF434343"/>
       <name val="Roboto"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12.0"/>
-      <color rgb="FF0F9D58"/>
-      <name val="Roboto"/>
-    </font>
-    <font>
-      <sz val="12.0"/>
-      <name val="Roboto"/>
-    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -632,7 +678,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="122">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -949,29 +995,45 @@
     <xf borderId="6" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="8" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
+    <xf borderId="6" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="4" fontId="13" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="5" fontId="13" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="5" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="6" fillId="5" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="5" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="4" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="6" fillId="5" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="6" fillId="4" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="10" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
     <dxf>
       <font/>
       <fill>
@@ -979,12 +1041,68 @@
       </fill>
       <border/>
     </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF3F3F3"/>
+          <bgColor rgb="FFF3F3F3"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
   </dxfs>
+  <tableStyles count="2">
+    <tableStyle count="2" pivot="0" name="Project Plan-style">
+      <tableStyleElement dxfId="1" type="firstRowStripe"/>
+      <tableStyleElement dxfId="2" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="2" pivot="0" name="Project Plan-style 2">
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="1" type="secondRowStripe"/>
+    </tableStyle>
+  </tableStyles>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="F41:J43" displayName="Table_1" id="1">
+  <tableColumns count="5">
+    <tableColumn name="Column1" id="1"/>
+    <tableColumn name="Column2" id="2"/>
+    <tableColumn name="Column3" id="3"/>
+    <tableColumn name="Column4" id="4"/>
+    <tableColumn name="Column5" id="5"/>
+  </tableColumns>
+  <tableStyleInfo name="Project Plan-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="F44:J44" displayName="Table_2" id="2">
+  <tableColumns count="5">
+    <tableColumn name="Column1" id="1"/>
+    <tableColumn name="Column2" id="2"/>
+    <tableColumn name="Column3" id="3"/>
+    <tableColumn name="Column4" id="4"/>
+    <tableColumn name="Column5" id="5"/>
+  </tableColumns>
+  <tableStyleInfo name="Project Plan-style 2" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2005,45 +2123,456 @@
     </row>
     <row r="32" ht="22.5" customHeight="1">
       <c r="A32" s="107"/>
-      <c r="B32" s="110"/>
-      <c r="C32" s="111"/>
-      <c r="D32" s="111"/>
-      <c r="E32" s="111"/>
-      <c r="F32" s="111"/>
-      <c r="G32" s="112"/>
-      <c r="H32" s="112"/>
-      <c r="I32" s="110"/>
-      <c r="J32" s="111"/>
-      <c r="K32" s="111"/>
-      <c r="L32" s="111"/>
-      <c r="M32" s="111"/>
-      <c r="N32" s="112"/>
-      <c r="O32" s="112"/>
-      <c r="P32" s="112"/>
-    </row>
-    <row r="33" ht="6.0" customHeight="1">
-      <c r="A33" s="113"/>
-      <c r="B33" s="114"/>
-      <c r="C33" s="113"/>
-      <c r="D33" s="113"/>
-      <c r="E33" s="113"/>
-      <c r="F33" s="113"/>
-      <c r="G33" s="113"/>
-      <c r="H33" s="113"/>
-      <c r="I33" s="113"/>
-      <c r="J33" s="115"/>
-      <c r="K33" s="115"/>
-      <c r="L33" s="113"/>
-      <c r="M33" s="113"/>
-      <c r="N33" s="113"/>
-      <c r="O33" s="113"/>
-      <c r="P33" s="113"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="39"/>
+      <c r="I32" s="39"/>
+      <c r="J32" s="39"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="P32" s="13"/>
+    </row>
+    <row r="33" ht="22.5" customHeight="1">
+      <c r="A33" s="107"/>
+      <c r="B33" s="10"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="K33" s="13"/>
+    </row>
+    <row r="34" ht="6.0" customHeight="1">
+      <c r="A34" s="110"/>
+      <c r="B34" s="75"/>
+      <c r="C34" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="F34" s="76" t="s">
+        <v>5</v>
+      </c>
+      <c r="G34" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="H34" s="76" t="s">
+        <v>7</v>
+      </c>
+      <c r="I34" s="76" t="s">
+        <v>8</v>
+      </c>
+      <c r="J34" s="76" t="s">
+        <v>9</v>
+      </c>
+      <c r="K34" s="76" t="s">
+        <v>10</v>
+      </c>
+      <c r="L34" s="77"/>
+      <c r="M34" s="77"/>
+      <c r="N34" s="77"/>
+      <c r="O34" s="78"/>
+      <c r="P34" s="78"/>
+    </row>
+    <row r="35" ht="6.0" customHeight="1">
+      <c r="A35" s="110"/>
+      <c r="B35" s="79" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="111" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" s="111" t="s">
+        <v>40</v>
+      </c>
+      <c r="E35" s="111" t="s">
+        <v>75</v>
+      </c>
+      <c r="F35" s="112">
+        <v>44265.0</v>
+      </c>
+      <c r="G35" s="112">
+        <v>44266.0</v>
+      </c>
+      <c r="H35" s="112">
+        <v>44265.0</v>
+      </c>
+      <c r="I35" s="112">
+        <v>44265.0</v>
+      </c>
+      <c r="J35" s="113">
+        <v>2.0</v>
+      </c>
+      <c r="K35" s="113">
+        <v>2.0</v>
+      </c>
+      <c r="L35" s="91"/>
+      <c r="M35" s="91"/>
+      <c r="N35" s="91"/>
+      <c r="O35" s="78"/>
+      <c r="P35" s="84"/>
+    </row>
+    <row r="36" ht="6.0" customHeight="1">
+      <c r="A36" s="110"/>
+      <c r="B36" s="85" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" s="80" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" s="80" t="s">
+        <v>77</v>
+      </c>
+      <c r="E36" s="80" t="s">
+        <v>78</v>
+      </c>
+      <c r="F36" s="114">
+        <v>44265.0</v>
+      </c>
+      <c r="G36" s="114">
+        <v>44266.0</v>
+      </c>
+      <c r="H36" s="114">
+        <v>44265.0</v>
+      </c>
+      <c r="I36" s="81"/>
+      <c r="J36" s="82">
+        <v>3.0</v>
+      </c>
+      <c r="K36" s="87"/>
+      <c r="L36" s="83"/>
+      <c r="M36" s="83"/>
+      <c r="N36" s="83"/>
+      <c r="O36" s="84"/>
+      <c r="P36" s="84"/>
+    </row>
+    <row r="37" ht="6.0" customHeight="1">
+      <c r="A37" s="110"/>
+      <c r="B37" s="85" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="111" t="s">
+        <v>79</v>
+      </c>
+      <c r="D37" s="111" t="s">
+        <v>80</v>
+      </c>
+      <c r="E37" s="111" t="s">
+        <v>81</v>
+      </c>
+      <c r="F37" s="112">
+        <v>44265.0</v>
+      </c>
+      <c r="G37" s="112">
+        <v>44266.0</v>
+      </c>
+      <c r="H37" s="112">
+        <v>44265.0</v>
+      </c>
+      <c r="I37" s="89"/>
+      <c r="J37" s="113">
+        <v>1.0</v>
+      </c>
+      <c r="K37" s="90"/>
+      <c r="L37" s="91"/>
+      <c r="M37" s="92"/>
+      <c r="N37" s="92"/>
+      <c r="O37" s="78"/>
+      <c r="P37" s="78"/>
+    </row>
+    <row r="38" ht="6.0" customHeight="1">
+      <c r="A38" s="110"/>
+      <c r="B38" s="85" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38" s="115" t="s">
+        <v>82</v>
+      </c>
+      <c r="D38" s="116" t="s">
+        <v>66</v>
+      </c>
+      <c r="E38" s="117" t="s">
+        <v>83</v>
+      </c>
+      <c r="F38" s="114">
+        <v>44265.0</v>
+      </c>
+      <c r="G38" s="114">
+        <v>44266.0</v>
+      </c>
+      <c r="H38" s="114">
+        <v>44265.0</v>
+      </c>
+      <c r="I38" s="81"/>
+      <c r="J38" s="82">
+        <v>1.0</v>
+      </c>
+      <c r="K38" s="87"/>
+      <c r="L38" s="84"/>
+      <c r="M38" s="84"/>
+      <c r="N38" s="84"/>
+      <c r="O38" s="84"/>
+      <c r="P38" s="84"/>
+    </row>
+    <row r="39" ht="6.0" customHeight="1">
+      <c r="A39" s="110"/>
+      <c r="B39" s="79" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39" s="80" t="s">
+        <v>84</v>
+      </c>
+      <c r="D39" s="80" t="s">
+        <v>85</v>
+      </c>
+      <c r="E39" s="80" t="s">
+        <v>86</v>
+      </c>
+      <c r="F39" s="114">
+        <v>44265.0</v>
+      </c>
+      <c r="G39" s="114">
+        <v>44266.0</v>
+      </c>
+      <c r="H39" s="114">
+        <v>44265.0</v>
+      </c>
+      <c r="I39" s="81"/>
+      <c r="J39" s="82">
+        <v>1.0</v>
+      </c>
+      <c r="K39" s="97"/>
+      <c r="L39" s="84"/>
+      <c r="M39" s="84"/>
+      <c r="N39" s="84"/>
+      <c r="O39" s="84"/>
+      <c r="P39" s="84"/>
+    </row>
+    <row r="40" ht="6.0" customHeight="1">
+      <c r="A40" s="110"/>
+      <c r="B40" s="79" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" s="118" t="s">
+        <v>54</v>
+      </c>
+      <c r="D40" s="113" t="s">
+        <v>87</v>
+      </c>
+      <c r="E40" s="113" t="s">
+        <v>88</v>
+      </c>
+      <c r="F40" s="112">
+        <v>44265.0</v>
+      </c>
+      <c r="G40" s="112">
+        <v>44266.0</v>
+      </c>
+      <c r="H40" s="112">
+        <v>44265.0</v>
+      </c>
+      <c r="I40" s="89"/>
+      <c r="J40" s="113">
+        <v>1.0</v>
+      </c>
+      <c r="K40" s="101"/>
+      <c r="L40" s="78"/>
+      <c r="M40" s="78"/>
+      <c r="N40" s="78"/>
+      <c r="O40" s="78"/>
+      <c r="P40" s="78"/>
+    </row>
+    <row r="41" ht="6.0" customHeight="1">
+      <c r="A41" s="110"/>
+      <c r="B41" s="79" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" s="86" t="s">
+        <v>47</v>
+      </c>
+      <c r="D41" s="87" t="s">
+        <v>62</v>
+      </c>
+      <c r="E41" s="87" t="s">
+        <v>63</v>
+      </c>
+      <c r="F41" s="114">
+        <v>44265.0</v>
+      </c>
+      <c r="G41" s="114">
+        <v>44266.0</v>
+      </c>
+      <c r="H41" s="114">
+        <v>44265.0</v>
+      </c>
+      <c r="I41" s="81"/>
+      <c r="J41" s="82">
+        <v>2.0</v>
+      </c>
+      <c r="K41" s="119"/>
+      <c r="L41" s="84"/>
+      <c r="M41" s="84"/>
+      <c r="N41" s="84"/>
+      <c r="O41" s="84"/>
+      <c r="P41" s="84"/>
+    </row>
+    <row r="42" ht="6.0" customHeight="1">
+      <c r="A42" s="110"/>
+      <c r="B42" s="79" t="s">
+        <v>55</v>
+      </c>
+      <c r="C42" s="120" t="s">
+        <v>89</v>
+      </c>
+      <c r="D42" s="113" t="s">
+        <v>72</v>
+      </c>
+      <c r="E42" s="113" t="s">
+        <v>72</v>
+      </c>
+      <c r="F42" s="112">
+        <v>44265.0</v>
+      </c>
+      <c r="G42" s="112">
+        <v>44266.0</v>
+      </c>
+      <c r="H42" s="112">
+        <v>44265.0</v>
+      </c>
+      <c r="I42" s="89"/>
+      <c r="J42" s="113">
+        <v>1.0</v>
+      </c>
+      <c r="K42" s="105"/>
+      <c r="L42" s="78"/>
+      <c r="M42" s="78"/>
+      <c r="N42" s="78"/>
+      <c r="O42" s="78"/>
+      <c r="P42" s="78"/>
+    </row>
+    <row r="43" ht="6.0" customHeight="1">
+      <c r="A43" s="110"/>
+      <c r="B43" s="79" t="s">
+        <v>58</v>
+      </c>
+      <c r="C43" s="80" t="s">
+        <v>90</v>
+      </c>
+      <c r="D43" s="82" t="s">
+        <v>91</v>
+      </c>
+      <c r="E43" s="82" t="s">
+        <v>91</v>
+      </c>
+      <c r="F43" s="114">
+        <v>44265.0</v>
+      </c>
+      <c r="G43" s="114">
+        <v>44266.0</v>
+      </c>
+      <c r="H43" s="114">
+        <v>44265.0</v>
+      </c>
+      <c r="I43" s="81"/>
+      <c r="J43" s="82">
+        <v>2.0</v>
+      </c>
+      <c r="K43" s="106"/>
+      <c r="L43" s="84"/>
+      <c r="M43" s="84"/>
+      <c r="N43" s="84"/>
+      <c r="O43" s="84"/>
+      <c r="P43" s="84"/>
+    </row>
+    <row r="44" ht="6.0" customHeight="1">
+      <c r="A44" s="110"/>
+      <c r="B44" s="79" t="s">
+        <v>71</v>
+      </c>
+      <c r="C44" s="118" t="s">
+        <v>82</v>
+      </c>
+      <c r="D44" s="113" t="s">
+        <v>92</v>
+      </c>
+      <c r="E44" s="113" t="s">
+        <v>92</v>
+      </c>
+      <c r="F44" s="112">
+        <v>44265.0</v>
+      </c>
+      <c r="G44" s="112">
+        <v>44266.0</v>
+      </c>
+      <c r="H44" s="112">
+        <v>44265.0</v>
+      </c>
+      <c r="I44" s="89"/>
+      <c r="J44" s="113">
+        <v>1.0</v>
+      </c>
+      <c r="K44" s="105"/>
+      <c r="L44" s="78"/>
+      <c r="M44" s="78"/>
+      <c r="N44" s="78"/>
+      <c r="O44" s="78"/>
+      <c r="P44" s="78"/>
+    </row>
+    <row r="45" ht="6.0" customHeight="1">
+      <c r="A45" s="110"/>
+      <c r="B45" s="85"/>
+      <c r="C45" s="86"/>
+      <c r="D45" s="121"/>
+      <c r="E45" s="121"/>
+      <c r="F45" s="121"/>
+      <c r="G45" s="121"/>
+      <c r="H45" s="121"/>
+      <c r="I45" s="121"/>
+      <c r="J45" s="121"/>
+      <c r="K45" s="106"/>
+      <c r="L45" s="84"/>
+      <c r="M45" s="84"/>
+      <c r="N45" s="84"/>
+      <c r="O45" s="84"/>
+      <c r="P45" s="84"/>
+    </row>
+    <row r="46" ht="6.0" customHeight="1">
+      <c r="A46" s="110"/>
+      <c r="B46" s="108"/>
+      <c r="C46" s="108"/>
+      <c r="D46" s="108"/>
+      <c r="E46" s="108"/>
+      <c r="F46" s="108"/>
+      <c r="G46" s="108"/>
+      <c r="H46" s="108"/>
+      <c r="I46" s="108"/>
+      <c r="J46" s="108"/>
+      <c r="K46" s="108"/>
+      <c r="L46" s="109"/>
+      <c r="M46" s="109"/>
+      <c r="N46" s="109"/>
+      <c r="O46" s="109"/>
+      <c r="P46" s="109"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="13">
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="F17:J17"/>
     <mergeCell ref="K17:P17"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="F33:J33"/>
+    <mergeCell ref="K33:P33"/>
     <mergeCell ref="F1:J1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:J2"/>
@@ -2054,5 +2583,9 @@
   </mergeCells>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updating the project plan according to the last changes
</commit_message>
<xml_diff>
--- a/SWE/SW deliveries log/PP/SWE_PO1_Digital_Calculator_ITI_41.xlsx
+++ b/SWE/SW deliveries log/PP/SWE_PO1_Digital_Calculator_ITI_41.xlsx
@@ -377,7 +377,7 @@
     <t xml:space="preserve">- Modify the CRS as per the last review </t>
   </si>
   <si>
-    <t xml:space="preserve">-Modify the HSI </t>
+    <t xml:space="preserve">-Modify the CRS </t>
   </si>
   <si>
     <t xml:space="preserve">-Add the lcd initilization sequence,and update the document as per the last review </t>
@@ -678,7 +678,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="123">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1021,6 +1021,9 @@
     </xf>
     <xf borderId="6" fillId="4" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="6" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="6" fillId="5" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2246,11 +2249,15 @@
       <c r="H36" s="114">
         <v>44265.0</v>
       </c>
-      <c r="I36" s="81"/>
+      <c r="I36" s="114">
+        <v>44265.0</v>
+      </c>
       <c r="J36" s="82">
         <v>3.0</v>
       </c>
-      <c r="K36" s="87"/>
+      <c r="K36" s="82">
+        <v>2.0</v>
+      </c>
       <c r="L36" s="83"/>
       <c r="M36" s="83"/>
       <c r="N36" s="83"/>
@@ -2280,7 +2287,9 @@
       <c r="H37" s="112">
         <v>44265.0</v>
       </c>
-      <c r="I37" s="89"/>
+      <c r="I37" s="112">
+        <v>44265.0</v>
+      </c>
       <c r="J37" s="113">
         <v>1.0</v>
       </c>
@@ -2314,7 +2323,9 @@
       <c r="H38" s="114">
         <v>44265.0</v>
       </c>
-      <c r="I38" s="81"/>
+      <c r="I38" s="114">
+        <v>44266.0</v>
+      </c>
       <c r="J38" s="82">
         <v>1.0</v>
       </c>
@@ -2348,7 +2359,9 @@
       <c r="H39" s="114">
         <v>44265.0</v>
       </c>
-      <c r="I39" s="81"/>
+      <c r="I39" s="114">
+        <v>44266.0</v>
+      </c>
       <c r="J39" s="82">
         <v>1.0</v>
       </c>
@@ -2367,10 +2380,10 @@
       <c r="C40" s="118" t="s">
         <v>54</v>
       </c>
-      <c r="D40" s="113" t="s">
+      <c r="D40" s="119" t="s">
         <v>87</v>
       </c>
-      <c r="E40" s="113" t="s">
+      <c r="E40" s="119" t="s">
         <v>88</v>
       </c>
       <c r="F40" s="112">
@@ -2382,7 +2395,9 @@
       <c r="H40" s="112">
         <v>44265.0</v>
       </c>
-      <c r="I40" s="89"/>
+      <c r="I40" s="112">
+        <v>44266.0</v>
+      </c>
       <c r="J40" s="113">
         <v>1.0</v>
       </c>
@@ -2401,10 +2416,10 @@
       <c r="C41" s="86" t="s">
         <v>47</v>
       </c>
-      <c r="D41" s="87" t="s">
+      <c r="D41" s="116" t="s">
         <v>62</v>
       </c>
-      <c r="E41" s="87" t="s">
+      <c r="E41" s="116" t="s">
         <v>63</v>
       </c>
       <c r="F41" s="114">
@@ -2420,7 +2435,7 @@
       <c r="J41" s="82">
         <v>2.0</v>
       </c>
-      <c r="K41" s="119"/>
+      <c r="K41" s="120"/>
       <c r="L41" s="84"/>
       <c r="M41" s="84"/>
       <c r="N41" s="84"/>
@@ -2432,13 +2447,13 @@
       <c r="B42" s="79" t="s">
         <v>55</v>
       </c>
-      <c r="C42" s="120" t="s">
+      <c r="C42" s="121" t="s">
         <v>89</v>
       </c>
-      <c r="D42" s="113" t="s">
+      <c r="D42" s="119" t="s">
         <v>72</v>
       </c>
-      <c r="E42" s="113" t="s">
+      <c r="E42" s="119" t="s">
         <v>72</v>
       </c>
       <c r="F42" s="112">
@@ -2450,7 +2465,9 @@
       <c r="H42" s="112">
         <v>44265.0</v>
       </c>
-      <c r="I42" s="89"/>
+      <c r="I42" s="112">
+        <v>44266.0</v>
+      </c>
       <c r="J42" s="113">
         <v>1.0</v>
       </c>
@@ -2469,10 +2486,10 @@
       <c r="C43" s="80" t="s">
         <v>90</v>
       </c>
-      <c r="D43" s="82" t="s">
+      <c r="D43" s="117" t="s">
         <v>91</v>
       </c>
-      <c r="E43" s="82" t="s">
+      <c r="E43" s="117" t="s">
         <v>91</v>
       </c>
       <c r="F43" s="114">
@@ -2484,7 +2501,9 @@
       <c r="H43" s="114">
         <v>44265.0</v>
       </c>
-      <c r="I43" s="81"/>
+      <c r="I43" s="114">
+        <v>44266.0</v>
+      </c>
       <c r="J43" s="82">
         <v>2.0</v>
       </c>
@@ -2503,10 +2522,10 @@
       <c r="C44" s="118" t="s">
         <v>82</v>
       </c>
-      <c r="D44" s="113" t="s">
+      <c r="D44" s="119" t="s">
         <v>92</v>
       </c>
-      <c r="E44" s="113" t="s">
+      <c r="E44" s="119" t="s">
         <v>92</v>
       </c>
       <c r="F44" s="112">
@@ -2518,7 +2537,9 @@
       <c r="H44" s="112">
         <v>44265.0</v>
       </c>
-      <c r="I44" s="89"/>
+      <c r="I44" s="112">
+        <v>44266.0</v>
+      </c>
       <c r="J44" s="113">
         <v>1.0</v>
       </c>
@@ -2533,13 +2554,13 @@
       <c r="A45" s="110"/>
       <c r="B45" s="85"/>
       <c r="C45" s="86"/>
-      <c r="D45" s="121"/>
-      <c r="E45" s="121"/>
-      <c r="F45" s="121"/>
-      <c r="G45" s="121"/>
-      <c r="H45" s="121"/>
-      <c r="I45" s="121"/>
-      <c r="J45" s="121"/>
+      <c r="D45" s="122"/>
+      <c r="E45" s="122"/>
+      <c r="F45" s="122"/>
+      <c r="G45" s="122"/>
+      <c r="H45" s="122"/>
+      <c r="I45" s="122"/>
+      <c r="J45" s="122"/>
       <c r="K45" s="106"/>
       <c r="L45" s="84"/>
       <c r="M45" s="84"/>

</xml_diff>